<commit_message>
updated names and export script
</commit_message>
<xml_diff>
--- a/daq_system/inputs/CMS_Master_Control_Wiring_Dev5.xlsx
+++ b/daq_system/inputs/CMS_Master_Control_Wiring_Dev5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmaso\Documents\DAQ\PSPL_DAQ\daq_system\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365D8EFD-8D31-4ED8-BC7D-D7666BA3D01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A9ED08-C61D-4498-AFA2-60D2B05CFDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>dev5/port0/line27</t>
   </si>
   <si>
-    <t>DELUGE</t>
-  </si>
-  <si>
     <t>IGNITOR</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>SV-N2-01</t>
+  </si>
+  <si>
+    <t>PV-WA-04</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1114,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -1290,7 +1290,7 @@
         <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -1302,10 +1302,10 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
@@ -1332,7 +1332,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
@@ -1346,10 +1346,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
         <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>36</v>
@@ -1374,10 +1374,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>

</xml_diff>